<commit_message>
add possibility to actually save new posts
</commit_message>
<xml_diff>
--- a/GradedExercise.xlsx
+++ b/GradedExercise.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gianm\IdeaProjects\hs18-enb-Lorius\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51BA22F-96C4-4BCB-AB51-1254481326D5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13860" yWindow="2260" windowWidth="30440" windowHeight="24580" tabRatio="500"/>
+    <workbookView xWindow="13860" yWindow="2260" windowWidth="30440" windowHeight="24580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,8 +18,15 @@
   <definedNames>
     <definedName name="TOTAL_POINTS">Sheet1!$I$33</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -165,11 +178,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -258,12 +271,20 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -588,14 +609,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="5.83203125" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>

</xml_diff>

<commit_message>
make a new branch to copy paste stuff from other branches into
</commit_message>
<xml_diff>
--- a/GradedExercise.xlsx
+++ b/GradedExercise.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gianm\IdeaProjects\hs18-enb-Lorius\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51BA22F-96C4-4BCB-AB51-1254481326D5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13860" yWindow="2260" windowWidth="30440" windowHeight="24580" tabRatio="500"/>
+    <workbookView xWindow="13860" yWindow="2260" windowWidth="30440" windowHeight="24580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,8 +18,15 @@
   <definedNames>
     <definedName name="TOTAL_POINTS">Sheet1!$I$33</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -165,11 +178,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -258,12 +271,20 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -588,14 +609,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="5.83203125" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>

</xml_diff>